<commit_message>
Update excel areas excel file
</commit_message>
<xml_diff>
--- a/data/darts-board-areas.xlsx
+++ b/data/darts-board-areas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3820190926b28df2/Personal projects/darts-monte-carlo-simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3820190926b28df2/Personal projects/darts-monte-carlo-simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="11_AD4DB114E441178AC67DF46F6655F10A693EDF23" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B239E124-91D9-449B-BF62-76641EFAB569}"/>
+  <xr:revisionPtr revIDLastSave="294" documentId="11_AD4DB114E441178AC67DF46F6655F10A693EDF23" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF1D34A6-E87E-45EB-936D-7B5D718D42AB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -36,20 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
-  <si>
-    <t>Board</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>Section</t>
   </si>
   <si>
-    <t>2x circle</t>
-  </si>
-  <si>
-    <t>3x circle</t>
-  </si>
-  <si>
     <t>Diameter</t>
   </si>
   <si>
@@ -59,38 +50,50 @@
     <t>Normalised area</t>
   </si>
   <si>
-    <t>Inner/outer</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>outer</t>
-  </si>
-  <si>
-    <t>inner</t>
-  </si>
-  <si>
     <t>Circle area</t>
   </si>
   <si>
     <t>Section area</t>
   </si>
   <si>
-    <t>Bullseye</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
+    <t>Total area smaller section (check)</t>
+  </si>
+  <si>
+    <t>Normalised area (%)</t>
+  </si>
+  <si>
+    <t>Outer bullseye</t>
+  </si>
+  <si>
+    <t>Inner bullseye</t>
+  </si>
+  <si>
+    <t>Inner circle</t>
+  </si>
+  <si>
+    <t>3x ring</t>
+  </si>
+  <si>
+    <t>middle circle</t>
+  </si>
+  <si>
+    <t>2x ring</t>
+  </si>
+  <si>
+    <t>outer board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,9 +102,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,57 +140,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="0"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{885D43F0-CC8A-4001-9042-7978933E32AA}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -185,26 +185,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A3F53C4-1B8B-4230-9F82-3D5D8A8992C6}" name="Table1" displayName="Table1" ref="A1:G8" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:G8" xr:uid="{2A3F53C4-1B8B-4230-9F82-3D5D8A8992C6}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B05E4868-20DA-42F9-8E7B-FA1D506DBC56}" name="Section"/>
-    <tableColumn id="2" xr3:uid="{DFA2128E-0A0F-4B4E-8218-F3E34D6BD647}" name="Inner/outer"/>
-    <tableColumn id="3" xr3:uid="{1A83DE1A-4996-4C16-9007-531607229D97}" name="Diameter" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{969C84A4-42F0-43A4-99D9-4FFBE45F4DD8}" name="Radius" dataDxfId="4">
-      <calculatedColumnFormula>C2/2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{DA8B1A6A-7030-458C-B0B5-CB7E2F6F86E4}" name="Circle area" dataDxfId="3">
-      <calculatedColumnFormula>D2^2*3.141592</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{E72D98E9-DD9F-4153-8FFF-E6EF2EE0F327}" name="Section area" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{0471EFEF-A013-417F-954D-CA218E811899}" name="Normalised area" dataDxfId="1">
-      <calculatedColumnFormula>F2/$F$10</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,250 +452,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>23.5</v>
-      </c>
-      <c r="D2" s="2">
-        <f>C2/2</f>
-        <v>11.75</v>
-      </c>
-      <c r="E2" s="2">
-        <f>D2^2*3.141592</f>
-        <v>433.73604550000005</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C2" s="5">
+        <f>B2/2</f>
+        <v>0.375</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D8" si="0">C2^2*3.141592</f>
+        <v>0.44178637500000001</v>
+      </c>
+      <c r="E2" s="1">
+        <f>D2</f>
+        <v>0.44178637500000001</v>
       </c>
       <c r="F2" s="2">
-        <f>E2-E3</f>
-        <v>179.26709350000004</v>
-      </c>
-      <c r="G2" s="3">
-        <f>F2/$F$10</f>
-        <v>0.33418618526286514</v>
+        <f>E2</f>
+        <v>0.44178637500000001</v>
+      </c>
+      <c r="G2" s="2">
+        <f>E2/$D$8</f>
+        <v>1.0185604345857853E-3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2">
-        <f t="shared" ref="D3:D8" si="0">C3/2</f>
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E8" si="1">D3^2*3.141592</f>
-        <v>254.468952</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="C3" s="5">
+        <f t="shared" ref="C3:C8" si="1">B3/2</f>
+        <v>0.875</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4052813749999999</v>
+      </c>
+      <c r="E3" s="1">
+        <f>D3-F2</f>
+        <v>1.963495</v>
       </c>
       <c r="F3" s="2">
-        <f>E3-E4</f>
-        <v>30.151429220000011</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G8" si="2">F3/$F$10</f>
-        <v>5.6207700557465032E-2</v>
+        <f>SUM($E$2:E3)</f>
+        <v>2.4052813749999999</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3/$D$8</f>
+        <v>4.5269352648257127E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="B4" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>8.4499999999999993</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="1"/>
-        <v>224.31752277999999</v>
+        <v>81.712807920000003</v>
+      </c>
+      <c r="E4" s="1">
+        <f>D4-F3</f>
+        <v>79.307526545000002</v>
       </c>
       <c r="F4" s="2">
-        <f>E4</f>
-        <v>224.31752277999999</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="2"/>
-        <v>0.41816830831512325</v>
+        <f>SUM($E$2:E4)</f>
+        <v>81.712807920000003</v>
+      </c>
+      <c r="G4" s="2">
+        <f>E4/$D$8</f>
+        <v>0.18284744228157535</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
         <v>11.3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="C5" s="5">
+        <f t="shared" si="1"/>
+        <v>5.65</v>
+      </c>
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>5.65</v>
-      </c>
-      <c r="E5" s="2">
+        <v>100.28747062000001</v>
+      </c>
+      <c r="E5" s="1">
+        <f>D5-F4</f>
+        <v>18.574662700000005</v>
+      </c>
+      <c r="F5" s="2">
+        <f>SUM($E$2:E5)</f>
+        <v>100.28747062000001</v>
+      </c>
+      <c r="G5" s="2">
+        <f>E5/$D$8</f>
+        <v>4.2824807605251251E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>100.28747062000001</v>
-      </c>
-      <c r="F5" s="2">
-        <f>E5-E6</f>
-        <v>18.574662700000005</v>
-      </c>
-      <c r="G5" s="3">
-        <f t="shared" si="2"/>
-        <v>3.4626520400730602E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D6" s="2">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="1"/>
-        <v>81.712807920000003</v>
+        <v>224.31752277999999</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ref="E6:E8" si="2">D6-F5</f>
+        <v>124.03005215999998</v>
       </c>
       <c r="F6" s="2">
-        <f>E6</f>
-        <v>81.712807920000003</v>
-      </c>
-      <c r="G6" s="3">
-        <f t="shared" si="2"/>
-        <v>0.15232740729353114</v>
+        <f>SUM($E$2:E6)</f>
+        <v>224.31752277999999</v>
+      </c>
+      <c r="G6" s="2">
+        <f>E6/$D$8</f>
+        <v>0.28595744680851054</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>254.468952</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>30.151429220000011</v>
+      </c>
+      <c r="F7" s="2">
+        <f>SUM($E$2:E7)</f>
+        <v>254.468952</v>
+      </c>
+      <c r="G7" s="2">
+        <f>E7/$D$8</f>
+        <v>6.9515617926663664E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="1"/>
+        <v>11.75</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>433.73604550000005</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>179.26709350000004</v>
+      </c>
+      <c r="F8" s="2">
+        <f>SUM($E$2:E8)</f>
+        <v>433.73604550000005</v>
+      </c>
+      <c r="G8" s="2">
+        <f>E8/$D$8</f>
+        <v>0.41330918967858765</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>0.75</v>
+      </c>
+      <c r="C13">
+        <v>0.375</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.44178637500000001</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.44178637500000001</v>
+      </c>
+      <c r="F13" s="6">
+        <f>G2*100</f>
+        <v>0.10185604345857853</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
         <v>1.75</v>
       </c>
-      <c r="D7" s="2">
-        <f t="shared" si="0"/>
+      <c r="C14">
         <v>0.875</v>
       </c>
-      <c r="E7" s="2">
-        <f t="shared" si="1"/>
+      <c r="D14" s="1">
         <v>2.4052813749999999</v>
       </c>
-      <c r="F7" s="2">
-        <f>E7-E8</f>
+      <c r="E14" s="1">
         <v>1.963495</v>
       </c>
-      <c r="G7" s="3">
-        <f t="shared" si="2"/>
-        <v>3.660308710436638E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="F14" s="6">
+        <f t="shared" ref="F14:F19" si="3">G3*100</f>
+        <v>0.45269352648257127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.375</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="1"/>
-        <v>0.44178637500000001</v>
-      </c>
-      <c r="F8" s="2">
-        <f>E8</f>
-        <v>0.44178637500000001</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="2"/>
-        <v>8.2356945984824359E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+      <c r="B15">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C15">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D15" s="1">
+        <v>81.712807920000003</v>
+      </c>
+      <c r="E15" s="1">
+        <v>79.307526545000002</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="3"/>
+        <v>18.284744228157535</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>11.3</v>
+      </c>
+      <c r="C16">
+        <v>5.65</v>
+      </c>
+      <c r="D16" s="1">
+        <v>100.28747062000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>18.574662700000005</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="3"/>
+        <v>4.2824807605251252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="C17">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="D17" s="1">
+        <v>224.31752277999999</v>
+      </c>
+      <c r="E17" s="1">
+        <v>124.03005215999998</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="3"/>
+        <v>28.595744680851055</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1">
+        <v>254.468952</v>
+      </c>
+      <c r="E18" s="1">
+        <v>30.151429220000011</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="3"/>
+        <v>6.9515617926663662</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F10" s="2">
-        <f>SUM(F2:F8)</f>
-        <v>536.42879749500003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B19">
+        <v>23.5</v>
+      </c>
+      <c r="C19">
+        <v>11.75</v>
+      </c>
+      <c r="D19" s="1">
+        <v>433.73604550000005</v>
+      </c>
+      <c r="E19" s="1">
+        <v>179.26709350000004</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="3"/>
+        <v>41.330918967858764</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>